<commit_message>
doc and picture updated
</commit_message>
<xml_diff>
--- a/perf_studies/db_streaming_perf.xlsx
+++ b/perf_studies/db_streaming_perf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cyetest\doc\perf_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE28085B-404C-4878-9816-C67A2F1F01E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFF952F-CE6C-454A-8B13-B6E8235B9AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27DC8368-7454-4141-A7E0-46C91157EB54}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Filter</t>
   </si>
@@ -73,6 +73,52 @@
   </si>
   <si>
     <t>Router/Freq 5 GHz</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Server:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ubuntu 20.04/MySQL 8.0.23/Acer Aspire 3, Intel® Core(TM) i5-1035G1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Client:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Win10 Family/Intel® Core™ i7-4770 CPU @ 3.40GHz x64</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -153,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -396,6 +442,17 @@
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
@@ -405,15 +462,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -422,10 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,32 +480,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -495,6 +519,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DC1397-4D0C-4519-B799-9C58B5D15247}">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,189 +919,213 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="1" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="15">
         <v>335</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <v>4964</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>296</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="13">
         <v>34230</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>6490</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="5">
         <v>32556</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="15">
         <v>503</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>4284</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <v>470</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="13">
         <v>36390</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="4">
         <v>7724</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="5">
         <v>37505</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="15">
         <v>692</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="2">
         <v>4875</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <v>679</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="13">
         <v>38063</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>16147</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="5">
         <v>43774</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="16">
         <v>3565</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="8">
         <v>22260</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="9">
         <v>5097</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="14">
         <v>69303</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="10">
         <v>65124</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="12">
         <v>85449</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="42">
         <v>1201</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30">
+      <c r="D9" s="43"/>
+      <c r="E9" s="43">
         <v>1533</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32">
+      <c r="F9" s="44"/>
+      <c r="G9" s="17">
         <v>18416</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="18">
         <v>147920</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="46"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B12:H12"/>
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:D3"/>

</xml_diff>